<commit_message>
updating filenames, including the logic for fewshot prompting
</commit_message>
<xml_diff>
--- a/times.xlsx
+++ b/times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhartnett/Documents/UniversityWork/Thesis/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ECDCD1-C68A-1642-8F9A-5B62668891CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF53390-8F94-F045-A490-82D560F3100F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44600" yWindow="19220" windowWidth="31400" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29740" yWindow="15100" windowWidth="34400" windowHeight="26360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$2:$A$26</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$2:$B$26</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$2:$A$26</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$2:$B$26</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -143,37 +140,10 @@
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0">
-      <cx:tx>
-        <cx:txData>
-          <cx:v>Model Runtimes</cx:v>
-        </cx:txData>
-      </cx:tx>
-      <cx:txPr>
-        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr" rtl="0">
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:sysClr>
-              </a:solidFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>Model Runtimes</a:t>
-          </a:r>
-        </a:p>
-      </cx:txPr>
-    </cx:title>
+    <cx:title pos="t" align="ctr" overlay="0"/>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{F29B0535-593B-E541-8FD5-74FB7FD8F209}">
+        <cx:series layoutId="boxWhisker" uniqueId="{32CD3F5F-5ADB-9B4C-8F8C-74C32942BFA3}">
           <cx:tx>
             <cx:txData>
               <cx:f>_xlchart.v1.1</cx:f>
@@ -760,16 +730,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -778,7 +748,7 @@
             <xdr:cNvPr id="2" name="Chart 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4990F5DB-A07B-DFAE-1DEC-6F76562657D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C16B656E-857B-81CF-DDBF-94C8EE81BBFD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -805,7 +775,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3092450" y="844550"/>
+              <a:off x="5010150" y="2622550"/>
               <a:ext cx="4572000" cy="2743200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1127,7 +1097,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>22.78</v>
+        <v>3.42</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1153,7 +1123,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>7.15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1161,7 +1131,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>23.22</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1169,7 +1139,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>14.11</v>
+        <v>15.18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1177,7 +1147,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>27.07</v>
+        <v>24.08</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1185,7 +1155,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>17.57</v>
+        <v>9.7799999999999994</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1193,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>5.61</v>
+        <v>2.84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -1201,7 +1171,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>39.78</v>
+        <v>9.0399999999999991</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1209,7 +1179,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>10.35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1217,7 +1187,7 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>18.079999999999998</v>
+        <v>17.41</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -1225,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>26.78</v>
+        <v>12.98</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -1233,7 +1203,7 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>7.93</v>
+        <v>15.21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -1241,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>26.15</v>
+        <v>3.68</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1249,7 +1219,7 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>31.3</v>
+        <v>30.88</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -1257,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <v>49.01</v>
+        <v>49.83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1265,7 +1235,7 @@
         <v>2</v>
       </c>
       <c r="B17">
-        <v>24.28</v>
+        <v>6.89</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1273,7 +1243,7 @@
         <v>3</v>
       </c>
       <c r="B18">
-        <v>7.5</v>
+        <v>6.94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -1281,7 +1251,7 @@
         <v>4</v>
       </c>
       <c r="B19">
-        <v>16.7</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1289,7 +1259,7 @@
         <v>5</v>
       </c>
       <c r="B20">
-        <v>12.21</v>
+        <v>12.72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -1297,7 +1267,7 @@
         <v>6</v>
       </c>
       <c r="B21">
-        <v>22.88</v>
+        <v>23.75</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1305,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>28.09</v>
+        <v>7.48</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1313,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="B23">
-        <v>8.9600000000000009</v>
+        <v>15.41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1321,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="B24">
-        <v>78.099999999999994</v>
+        <v>3.63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -1329,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="B25">
-        <v>16.920000000000002</v>
+        <v>16.86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -1337,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="B26">
-        <v>28.76</v>
+        <v>28.61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>